<commit_message>
Fixes casing issue for offshore in disbursements file
</commit_message>
<xml_diff>
--- a/downloads/disbursements/disbursements.xlsx
+++ b/downloads/disbursements/disbursements.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malcolmj\Documents\GitHub\doi-extractives-data\gatsby-site\src\data-graphql\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnsobr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6067" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6067" uniqueCount="264">
   <si>
     <t>Fiscal Year</t>
   </si>
@@ -787,9 +787,6 @@
     <t>Gunnison County</t>
   </si>
   <si>
-    <t>offshore</t>
-  </si>
-  <si>
     <t>St Bernard Parish</t>
   </si>
   <si>
@@ -1251,25 +1248,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1704"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1292" workbookViewId="0">
-      <selection activeCell="H1303" sqref="H1303"/>
+    <sheetView tabSelected="1" topLeftCell="A1406" workbookViewId="0">
+      <selection activeCell="C1441" sqref="C1441"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" customWidth="1"/>
-    <col min="10" max="26" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" customWidth="1"/>
+    <col min="10" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="14.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1289,7 +1286,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="14.4">
       <c r="A2" s="5">
         <v>2003</v>
       </c>
@@ -1305,7 +1302,7 @@
         <v>224798713.59999999</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="14.4">
       <c r="A3" s="5">
         <v>2003</v>
       </c>
@@ -1321,7 +1318,7 @@
         <v>150000000</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" ht="14.4">
       <c r="A4" s="5">
         <v>2003</v>
       </c>
@@ -1337,7 +1334,7 @@
         <v>898999960</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" ht="14.4">
       <c r="A5" s="5">
         <v>2003</v>
       </c>
@@ -1353,7 +1350,7 @@
         <v>753373594.29999995</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="14.4">
       <c r="A6" s="5">
         <v>2003</v>
       </c>
@@ -1371,7 +1368,7 @@
         <v>529848.84</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" ht="14.4">
       <c r="A7" s="5">
         <v>2003</v>
       </c>
@@ -1389,7 +1386,7 @@
         <v>9030501.7400000002</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" ht="14.4">
       <c r="A8" s="5">
         <v>2003</v>
       </c>
@@ -1407,7 +1404,7 @@
         <v>121898.09</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" ht="14.4">
       <c r="A9" s="5">
         <v>2003</v>
       </c>
@@ -1425,7 +1422,7 @@
         <v>4108480.76</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="14.4">
       <c r="A10" s="5">
         <v>2003</v>
       </c>
@@ -1443,7 +1440,7 @@
         <v>21837849.16</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="14.4">
       <c r="A11" s="5">
         <v>2003</v>
       </c>
@@ -1461,7 +1458,7 @@
         <v>53947136.920000002</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" ht="14.4">
       <c r="A12" s="5">
         <v>2003</v>
       </c>
@@ -1479,7 +1476,7 @@
         <v>368710.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" ht="14.4">
       <c r="A13" s="5">
         <v>2003</v>
       </c>
@@ -1497,7 +1494,7 @@
         <v>1792864.42</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="14.4">
       <c r="A14" s="5">
         <v>2003</v>
       </c>
@@ -1515,7 +1512,7 @@
         <v>109312.47</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" ht="14.4">
       <c r="A15" s="5">
         <v>2003</v>
       </c>
@@ -1533,7 +1530,7 @@
         <v>6379.25</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" ht="14.4">
       <c r="A16" s="5">
         <v>2003</v>
       </c>
@@ -1551,7 +1548,7 @@
         <v>1823378.27</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" ht="14.4">
       <c r="A17" s="5">
         <v>2003</v>
       </c>
@@ -1569,7 +1566,7 @@
         <v>50131.79</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" ht="14.4">
       <c r="A18" s="5">
         <v>2003</v>
       </c>
@@ -1587,7 +1584,7 @@
         <v>1182451.3700000001</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" ht="14.4">
       <c r="A19" s="5">
         <v>2003</v>
       </c>
@@ -1605,7 +1602,7 @@
         <v>430602.31</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" ht="14.4">
       <c r="A20" s="5">
         <v>2003</v>
       </c>
@@ -28442,7 +28439,7 @@
         <v>60</v>
       </c>
       <c r="C1441" s="19" t="s">
-        <v>255</v>
+        <v>61</v>
       </c>
       <c r="D1441" s="6"/>
       <c r="E1441" s="19"/>
@@ -30094,7 +30091,7 @@
         <v>68</v>
       </c>
       <c r="E1528" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F1528" s="20">
         <v>3630.18</v>
@@ -30114,7 +30111,7 @@
         <v>68</v>
       </c>
       <c r="E1529" s="19" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F1529" s="20">
         <v>2600</v>
@@ -30134,7 +30131,7 @@
         <v>68</v>
       </c>
       <c r="E1530" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F1530" s="20">
         <v>2180.4</v>
@@ -30154,7 +30151,7 @@
         <v>68</v>
       </c>
       <c r="E1531" s="19" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F1531" s="20">
         <v>2397.81</v>
@@ -30174,7 +30171,7 @@
         <v>68</v>
       </c>
       <c r="E1532" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F1532" s="20">
         <v>2317.1899999999996</v>
@@ -30194,7 +30191,7 @@
         <v>68</v>
       </c>
       <c r="E1533" s="19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F1533" s="20">
         <v>2375.9499999999998</v>
@@ -30214,7 +30211,7 @@
         <v>68</v>
       </c>
       <c r="E1534" s="19" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F1534" s="20">
         <v>4089.9800000000005</v>
@@ -30762,7 +30759,7 @@
         <v>166</v>
       </c>
       <c r="C1562" s="14" t="s">
-        <v>255</v>
+        <v>61</v>
       </c>
       <c r="D1562" s="6" t="s">
         <v>17</v>
@@ -30780,7 +30777,7 @@
         <v>166</v>
       </c>
       <c r="C1563" s="14" t="s">
-        <v>255</v>
+        <v>61</v>
       </c>
       <c r="D1563" s="6" t="s">
         <v>15</v>
@@ -30798,7 +30795,7 @@
         <v>166</v>
       </c>
       <c r="C1564" s="14" t="s">
-        <v>255</v>
+        <v>61</v>
       </c>
       <c r="D1564" s="6" t="s">
         <v>30</v>
@@ -30816,7 +30813,7 @@
         <v>166</v>
       </c>
       <c r="C1565" s="14" t="s">
-        <v>255</v>
+        <v>61</v>
       </c>
       <c r="D1565" s="6" t="s">
         <v>68</v>
@@ -30834,7 +30831,7 @@
         <v>166</v>
       </c>
       <c r="C1566" s="14" t="s">
-        <v>255</v>
+        <v>61</v>
       </c>
       <c r="D1566" s="6" t="s">
         <v>71</v>
@@ -30852,7 +30849,7 @@
         <v>166</v>
       </c>
       <c r="C1567" s="14" t="s">
-        <v>255</v>
+        <v>61</v>
       </c>
       <c r="D1567" s="6" t="s">
         <v>85</v>
@@ -30870,7 +30867,7 @@
         <v>166</v>
       </c>
       <c r="C1568" s="14" t="s">
-        <v>255</v>
+        <v>61</v>
       </c>
       <c r="D1568" s="6" t="s">
         <v>133</v>
@@ -30888,7 +30885,7 @@
         <v>166</v>
       </c>
       <c r="C1569" s="14" t="s">
-        <v>255</v>
+        <v>61</v>
       </c>
       <c r="D1569" s="6" t="s">
         <v>145</v>
@@ -30958,7 +30955,7 @@
       </c>
       <c r="D1573" s="6"/>
       <c r="E1573" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1573" s="7">
         <v>1022539457.2899991</v>
@@ -30976,7 +30973,7 @@
       </c>
       <c r="D1574" s="6"/>
       <c r="E1574" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1574" s="7">
         <v>150000000</v>
@@ -30994,7 +30991,7 @@
       </c>
       <c r="D1575" s="6"/>
       <c r="E1575" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1575" s="7">
         <v>893887297</v>
@@ -31005,14 +31002,14 @@
         <v>2018</v>
       </c>
       <c r="B1576" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C1576" s="6" t="s">
         <v>61</v>
       </c>
       <c r="D1576" s="6"/>
       <c r="E1576" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1576" s="7">
         <v>76357901.970000029</v>
@@ -31030,7 +31027,7 @@
       </c>
       <c r="D1577" s="6"/>
       <c r="E1577" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1577" s="7">
         <v>116875634.66</v>
@@ -31048,7 +31045,7 @@
       </c>
       <c r="D1578" s="6"/>
       <c r="E1578" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1578" s="7">
         <v>163170752.99000001</v>
@@ -31066,7 +31063,7 @@
       </c>
       <c r="D1579" s="6"/>
       <c r="E1579" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1579" s="7">
         <v>1221259347.2999983</v>
@@ -31086,7 +31083,7 @@
         <v>17</v>
       </c>
       <c r="E1580" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1580" s="7">
         <v>1376095.1500000001</v>
@@ -31106,7 +31103,7 @@
         <v>15</v>
       </c>
       <c r="E1581" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1581" s="7">
         <v>34370934.209999993</v>
@@ -31126,7 +31123,7 @@
         <v>25</v>
       </c>
       <c r="E1582" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1582" s="7">
         <v>9069.7200000000012</v>
@@ -31146,7 +31143,7 @@
         <v>21</v>
       </c>
       <c r="E1583" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1583" s="7">
         <v>854176.1599999998</v>
@@ -31166,7 +31163,7 @@
         <v>30</v>
       </c>
       <c r="E1584" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1584" s="7">
         <v>41429712.409999996</v>
@@ -31346,7 +31343,7 @@
         <v>34</v>
       </c>
       <c r="E1593" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1593" s="7">
         <v>112554166.89000006</v>
@@ -31406,7 +31403,7 @@
         <v>44</v>
       </c>
       <c r="E1596" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1596" s="7">
         <v>476560.88</v>
@@ -31426,7 +31423,7 @@
         <v>55</v>
       </c>
       <c r="E1597" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1597" s="7">
         <v>4333975.8100000005</v>
@@ -31526,7 +31523,7 @@
         <v>57</v>
       </c>
       <c r="E1602" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1602" s="7">
         <v>76415.92</v>
@@ -31546,7 +31543,7 @@
         <v>59</v>
       </c>
       <c r="E1603" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1603" s="7">
         <v>3693.9700000000003</v>
@@ -31566,7 +31563,7 @@
         <v>63</v>
       </c>
       <c r="E1604" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1604" s="7">
         <v>639045.52000000025</v>
@@ -31586,7 +31583,7 @@
         <v>66</v>
       </c>
       <c r="E1605" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1605" s="7">
         <v>120512.24</v>
@@ -31606,7 +31603,7 @@
         <v>68</v>
       </c>
       <c r="E1606" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1606" s="7">
         <v>2153237.5400000005</v>
@@ -31626,7 +31623,7 @@
         <v>79</v>
       </c>
       <c r="E1607" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1607" s="7">
         <v>147823.25</v>
@@ -31646,7 +31643,7 @@
         <v>81</v>
       </c>
       <c r="E1608" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1608" s="7">
         <v>11554.300000000001</v>
@@ -31666,7 +31663,7 @@
         <v>85</v>
       </c>
       <c r="E1609" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1609" s="7">
         <v>661429.36999999988</v>
@@ -31686,7 +31683,7 @@
         <v>83</v>
       </c>
       <c r="E1610" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1610" s="7">
         <v>2299269.8000000003</v>
@@ -31706,7 +31703,7 @@
         <v>87</v>
       </c>
       <c r="E1611" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1611" s="7">
         <v>25686291.770000052</v>
@@ -31726,7 +31723,7 @@
         <v>97</v>
       </c>
       <c r="E1612" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1612" s="7">
         <v>28700.580000000005</v>
@@ -31746,7 +31743,7 @@
         <v>113</v>
       </c>
       <c r="E1613" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1613" s="7">
         <v>4066416.8100000015</v>
@@ -32006,7 +32003,7 @@
         <v>105</v>
       </c>
       <c r="E1626" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1626" s="7">
         <v>634977556.71000016</v>
@@ -32066,7 +32063,7 @@
         <v>95</v>
       </c>
       <c r="E1629" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1629" s="7">
         <v>53223774.739999957</v>
@@ -32086,7 +32083,7 @@
         <v>117</v>
       </c>
       <c r="E1630" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1630" s="7">
         <v>862521.52000000025</v>
@@ -32106,7 +32103,7 @@
         <v>119</v>
       </c>
       <c r="E1631" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1631" s="7">
         <v>7867081.6499999939</v>
@@ -32126,7 +32123,7 @@
         <v>123</v>
       </c>
       <c r="E1632" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1632" s="7">
         <v>47141.71</v>
@@ -32186,7 +32183,7 @@
         <v>125</v>
       </c>
       <c r="E1635" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1635" s="7">
         <v>9880.119999999999</v>
@@ -32206,7 +32203,7 @@
         <v>135</v>
       </c>
       <c r="E1636" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1636" s="7">
         <v>518.37</v>
@@ -32226,7 +32223,7 @@
         <v>137</v>
       </c>
       <c r="E1637" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1637" s="7">
         <v>564521.81999999983</v>
@@ -32246,7 +32243,7 @@
         <v>145</v>
       </c>
       <c r="E1638" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1638" s="7">
         <v>4847388.660000002</v>
@@ -32266,7 +32263,7 @@
         <v>149</v>
       </c>
       <c r="E1639" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1639" s="7">
         <v>76015357.680000067</v>
@@ -32366,7 +32363,7 @@
         <v>151</v>
       </c>
       <c r="E1644" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1644" s="7">
         <v>39194.81</v>
@@ -32386,7 +32383,7 @@
         <v>157</v>
       </c>
       <c r="E1645" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1645" s="7">
         <v>7999.7800000000007</v>
@@ -32426,7 +32423,7 @@
         <v>161</v>
       </c>
       <c r="E1647" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1647" s="7">
         <v>470583.49000000017</v>
@@ -32446,7 +32443,7 @@
         <v>159</v>
       </c>
       <c r="E1648" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1648" s="7">
         <v>233.5</v>
@@ -32466,7 +32463,7 @@
         <v>163</v>
       </c>
       <c r="E1649" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1649" s="7">
         <v>563955987.69999945</v>
@@ -32724,7 +32721,7 @@
         <v>68</v>
       </c>
       <c r="E1662" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F1662" s="7">
         <v>781611.41</v>
@@ -32744,7 +32741,7 @@
         <v>68</v>
       </c>
       <c r="E1663" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F1663" s="7">
         <v>594151.57999999996</v>
@@ -32764,7 +32761,7 @@
         <v>68</v>
       </c>
       <c r="E1664" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F1664" s="7">
         <v>517254.38000000006</v>
@@ -32784,7 +32781,7 @@
         <v>68</v>
       </c>
       <c r="E1665" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F1665" s="7">
         <v>559530.88</v>
@@ -32804,7 +32801,7 @@
         <v>68</v>
       </c>
       <c r="E1666" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F1666" s="7">
         <v>616852.85</v>
@@ -32824,7 +32821,7 @@
         <v>68</v>
       </c>
       <c r="E1667" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F1667" s="7">
         <v>719952.25</v>
@@ -32844,7 +32841,7 @@
         <v>68</v>
       </c>
       <c r="E1668" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F1668" s="7">
         <v>912548.87</v>
@@ -33398,7 +33395,7 @@
         <v>17</v>
       </c>
       <c r="E1696" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1696" s="7">
         <v>2384757.73</v>
@@ -33418,7 +33415,7 @@
         <v>15</v>
       </c>
       <c r="E1697" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1697" s="7">
         <v>1509923.7600000002</v>
@@ -33438,7 +33435,7 @@
         <v>30</v>
       </c>
       <c r="E1698" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1698" s="7">
         <v>1363323.5800000008</v>
@@ -33458,7 +33455,7 @@
         <v>68</v>
       </c>
       <c r="E1699" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1699" s="7">
         <v>6052631.0099999998</v>
@@ -33478,7 +33475,7 @@
         <v>85</v>
       </c>
       <c r="E1700" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1700" s="7">
         <v>259421.05999999994</v>
@@ -33498,7 +33495,7 @@
         <v>145</v>
       </c>
       <c r="E1701" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1701" s="7">
         <v>4634850.8399999961</v>
@@ -33516,7 +33513,7 @@
       </c>
       <c r="D1702" s="6"/>
       <c r="E1702" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1702" s="7">
         <v>2789421770.9399981</v>
@@ -33534,7 +33531,7 @@
       </c>
       <c r="D1703" s="6"/>
       <c r="E1703" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1703" s="7">
         <v>411828484.52999961</v>
@@ -33552,7 +33549,7 @@
       </c>
       <c r="D1704" s="6"/>
       <c r="E1704" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1704" s="7">
         <v>309064093.10999995</v>
@@ -33570,13 +33567,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="14.4">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -33584,7 +33581,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30">
+    <row r="2" spans="1:2" ht="27.6">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -33592,7 +33589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="14.4">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -33600,7 +33597,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30">
+    <row r="4" spans="1:2" ht="27.6">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -33608,7 +33605,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="14.4">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -33616,7 +33613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="14.4">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -33624,7 +33621,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30">
+    <row r="7" spans="1:2" ht="27.6">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -33632,7 +33629,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="14.4">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
@@ -33640,7 +33637,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="14.4">
       <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
@@ -33648,7 +33645,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" ht="14.4">
       <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
@@ -33656,7 +33653,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="14.4">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
@@ -33664,7 +33661,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="14.4">
       <c r="A12" s="4" t="s">
         <v>29</v>
       </c>
@@ -33672,7 +33669,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="14.4">
       <c r="A13" s="4" t="s">
         <v>31</v>
       </c>
@@ -33680,7 +33677,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" ht="14.4">
       <c r="A14" s="4" t="s">
         <v>33</v>
       </c>
@@ -33688,7 +33685,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" ht="14.4">
       <c r="A15" s="4" t="s">
         <v>35</v>
       </c>
@@ -33696,7 +33693,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="14.4">
       <c r="A16" s="4" t="s">
         <v>37</v>
       </c>
@@ -33704,7 +33701,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="14.4">
       <c r="A17" s="4" t="s">
         <v>39</v>
       </c>
@@ -33712,7 +33709,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" ht="14.4">
       <c r="A18" s="4" t="s">
         <v>41</v>
       </c>
@@ -33720,7 +33717,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" ht="14.4">
       <c r="A19" s="4" t="s">
         <v>43</v>
       </c>
@@ -33728,7 +33725,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" ht="14.4">
       <c r="A20" s="4" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Fixes capitalization for offshore
</commit_message>
<xml_diff>
--- a/downloads/disbursements/disbursements.xlsx
+++ b/downloads/disbursements/disbursements.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malcolmj\Documents\GitHub\doi-extractives-data\gatsby-site\src\data-graphql\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\doi-extractives-data\downloads\disbursements\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6067" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6067" uniqueCount="264">
   <si>
     <t>Fiscal Year</t>
   </si>
@@ -787,9 +787,6 @@
     <t>Gunnison County</t>
   </si>
   <si>
-    <t>offshore</t>
-  </si>
-  <si>
     <t>St Bernard Parish</t>
   </si>
   <si>
@@ -1251,25 +1248,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1704"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1292" workbookViewId="0">
-      <selection activeCell="H1303" sqref="H1303"/>
+    <sheetView tabSelected="1" topLeftCell="A1406" workbookViewId="0">
+      <selection activeCell="C1441" sqref="C1441"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" customWidth="1"/>
-    <col min="10" max="26" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" customWidth="1"/>
+    <col min="10" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="14.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1289,7 +1286,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="14.4">
       <c r="A2" s="5">
         <v>2003</v>
       </c>
@@ -1305,7 +1302,7 @@
         <v>224798713.59999999</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="14.4">
       <c r="A3" s="5">
         <v>2003</v>
       </c>
@@ -1321,7 +1318,7 @@
         <v>150000000</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" ht="14.4">
       <c r="A4" s="5">
         <v>2003</v>
       </c>
@@ -1337,7 +1334,7 @@
         <v>898999960</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" ht="14.4">
       <c r="A5" s="5">
         <v>2003</v>
       </c>
@@ -1353,7 +1350,7 @@
         <v>753373594.29999995</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="14.4">
       <c r="A6" s="5">
         <v>2003</v>
       </c>
@@ -1371,7 +1368,7 @@
         <v>529848.84</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" ht="14.4">
       <c r="A7" s="5">
         <v>2003</v>
       </c>
@@ -1389,7 +1386,7 @@
         <v>9030501.7400000002</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" ht="14.4">
       <c r="A8" s="5">
         <v>2003</v>
       </c>
@@ -1407,7 +1404,7 @@
         <v>121898.09</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" ht="14.4">
       <c r="A9" s="5">
         <v>2003</v>
       </c>
@@ -1425,7 +1422,7 @@
         <v>4108480.76</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="14.4">
       <c r="A10" s="5">
         <v>2003</v>
       </c>
@@ -1443,7 +1440,7 @@
         <v>21837849.16</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="14.4">
       <c r="A11" s="5">
         <v>2003</v>
       </c>
@@ -1461,7 +1458,7 @@
         <v>53947136.920000002</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" ht="14.4">
       <c r="A12" s="5">
         <v>2003</v>
       </c>
@@ -1479,7 +1476,7 @@
         <v>368710.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" ht="14.4">
       <c r="A13" s="5">
         <v>2003</v>
       </c>
@@ -1497,7 +1494,7 @@
         <v>1792864.42</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="14.4">
       <c r="A14" s="5">
         <v>2003</v>
       </c>
@@ -1515,7 +1512,7 @@
         <v>109312.47</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" ht="14.4">
       <c r="A15" s="5">
         <v>2003</v>
       </c>
@@ -1533,7 +1530,7 @@
         <v>6379.25</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" ht="14.4">
       <c r="A16" s="5">
         <v>2003</v>
       </c>
@@ -1551,7 +1548,7 @@
         <v>1823378.27</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" ht="14.4">
       <c r="A17" s="5">
         <v>2003</v>
       </c>
@@ -1569,7 +1566,7 @@
         <v>50131.79</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" ht="14.4">
       <c r="A18" s="5">
         <v>2003</v>
       </c>
@@ -1587,7 +1584,7 @@
         <v>1182451.3700000001</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" ht="14.4">
       <c r="A19" s="5">
         <v>2003</v>
       </c>
@@ -1605,7 +1602,7 @@
         <v>430602.31</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" ht="14.4">
       <c r="A20" s="5">
         <v>2003</v>
       </c>
@@ -28442,7 +28439,7 @@
         <v>60</v>
       </c>
       <c r="C1441" s="19" t="s">
-        <v>255</v>
+        <v>61</v>
       </c>
       <c r="D1441" s="6"/>
       <c r="E1441" s="19"/>
@@ -30094,7 +30091,7 @@
         <v>68</v>
       </c>
       <c r="E1528" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F1528" s="20">
         <v>3630.18</v>
@@ -30114,7 +30111,7 @@
         <v>68</v>
       </c>
       <c r="E1529" s="19" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F1529" s="20">
         <v>2600</v>
@@ -30134,7 +30131,7 @@
         <v>68</v>
       </c>
       <c r="E1530" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F1530" s="20">
         <v>2180.4</v>
@@ -30154,7 +30151,7 @@
         <v>68</v>
       </c>
       <c r="E1531" s="19" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F1531" s="20">
         <v>2397.81</v>
@@ -30174,7 +30171,7 @@
         <v>68</v>
       </c>
       <c r="E1532" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F1532" s="20">
         <v>2317.1899999999996</v>
@@ -30194,7 +30191,7 @@
         <v>68</v>
       </c>
       <c r="E1533" s="19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F1533" s="20">
         <v>2375.9499999999998</v>
@@ -30214,7 +30211,7 @@
         <v>68</v>
       </c>
       <c r="E1534" s="19" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F1534" s="20">
         <v>4089.9800000000005</v>
@@ -30762,7 +30759,7 @@
         <v>166</v>
       </c>
       <c r="C1562" s="14" t="s">
-        <v>255</v>
+        <v>61</v>
       </c>
       <c r="D1562" s="6" t="s">
         <v>17</v>
@@ -30780,7 +30777,7 @@
         <v>166</v>
       </c>
       <c r="C1563" s="14" t="s">
-        <v>255</v>
+        <v>61</v>
       </c>
       <c r="D1563" s="6" t="s">
         <v>15</v>
@@ -30798,7 +30795,7 @@
         <v>166</v>
       </c>
       <c r="C1564" s="14" t="s">
-        <v>255</v>
+        <v>61</v>
       </c>
       <c r="D1564" s="6" t="s">
         <v>30</v>
@@ -30816,7 +30813,7 @@
         <v>166</v>
       </c>
       <c r="C1565" s="14" t="s">
-        <v>255</v>
+        <v>61</v>
       </c>
       <c r="D1565" s="6" t="s">
         <v>68</v>
@@ -30834,7 +30831,7 @@
         <v>166</v>
       </c>
       <c r="C1566" s="14" t="s">
-        <v>255</v>
+        <v>61</v>
       </c>
       <c r="D1566" s="6" t="s">
         <v>71</v>
@@ -30852,7 +30849,7 @@
         <v>166</v>
       </c>
       <c r="C1567" s="14" t="s">
-        <v>255</v>
+        <v>61</v>
       </c>
       <c r="D1567" s="6" t="s">
         <v>85</v>
@@ -30870,7 +30867,7 @@
         <v>166</v>
       </c>
       <c r="C1568" s="14" t="s">
-        <v>255</v>
+        <v>61</v>
       </c>
       <c r="D1568" s="6" t="s">
         <v>133</v>
@@ -30888,7 +30885,7 @@
         <v>166</v>
       </c>
       <c r="C1569" s="14" t="s">
-        <v>255</v>
+        <v>61</v>
       </c>
       <c r="D1569" s="6" t="s">
         <v>145</v>
@@ -30958,7 +30955,7 @@
       </c>
       <c r="D1573" s="6"/>
       <c r="E1573" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1573" s="7">
         <v>1022539457.2899991</v>
@@ -30976,7 +30973,7 @@
       </c>
       <c r="D1574" s="6"/>
       <c r="E1574" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1574" s="7">
         <v>150000000</v>
@@ -30994,7 +30991,7 @@
       </c>
       <c r="D1575" s="6"/>
       <c r="E1575" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1575" s="7">
         <v>893887297</v>
@@ -31005,14 +31002,14 @@
         <v>2018</v>
       </c>
       <c r="B1576" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C1576" s="6" t="s">
         <v>61</v>
       </c>
       <c r="D1576" s="6"/>
       <c r="E1576" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1576" s="7">
         <v>76357901.970000029</v>
@@ -31030,7 +31027,7 @@
       </c>
       <c r="D1577" s="6"/>
       <c r="E1577" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1577" s="7">
         <v>116875634.66</v>
@@ -31048,7 +31045,7 @@
       </c>
       <c r="D1578" s="6"/>
       <c r="E1578" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1578" s="7">
         <v>163170752.99000001</v>
@@ -31066,7 +31063,7 @@
       </c>
       <c r="D1579" s="6"/>
       <c r="E1579" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1579" s="7">
         <v>1221259347.2999983</v>
@@ -31086,7 +31083,7 @@
         <v>17</v>
       </c>
       <c r="E1580" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1580" s="7">
         <v>1376095.1500000001</v>
@@ -31106,7 +31103,7 @@
         <v>15</v>
       </c>
       <c r="E1581" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1581" s="7">
         <v>34370934.209999993</v>
@@ -31126,7 +31123,7 @@
         <v>25</v>
       </c>
       <c r="E1582" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1582" s="7">
         <v>9069.7200000000012</v>
@@ -31146,7 +31143,7 @@
         <v>21</v>
       </c>
       <c r="E1583" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1583" s="7">
         <v>854176.1599999998</v>
@@ -31166,7 +31163,7 @@
         <v>30</v>
       </c>
       <c r="E1584" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1584" s="7">
         <v>41429712.409999996</v>
@@ -31346,7 +31343,7 @@
         <v>34</v>
       </c>
       <c r="E1593" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1593" s="7">
         <v>112554166.89000006</v>
@@ -31406,7 +31403,7 @@
         <v>44</v>
       </c>
       <c r="E1596" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1596" s="7">
         <v>476560.88</v>
@@ -31426,7 +31423,7 @@
         <v>55</v>
       </c>
       <c r="E1597" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1597" s="7">
         <v>4333975.8100000005</v>
@@ -31526,7 +31523,7 @@
         <v>57</v>
       </c>
       <c r="E1602" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1602" s="7">
         <v>76415.92</v>
@@ -31546,7 +31543,7 @@
         <v>59</v>
       </c>
       <c r="E1603" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1603" s="7">
         <v>3693.9700000000003</v>
@@ -31566,7 +31563,7 @@
         <v>63</v>
       </c>
       <c r="E1604" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1604" s="7">
         <v>639045.52000000025</v>
@@ -31586,7 +31583,7 @@
         <v>66</v>
       </c>
       <c r="E1605" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1605" s="7">
         <v>120512.24</v>
@@ -31606,7 +31603,7 @@
         <v>68</v>
       </c>
       <c r="E1606" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1606" s="7">
         <v>2153237.5400000005</v>
@@ -31626,7 +31623,7 @@
         <v>79</v>
       </c>
       <c r="E1607" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1607" s="7">
         <v>147823.25</v>
@@ -31646,7 +31643,7 @@
         <v>81</v>
       </c>
       <c r="E1608" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1608" s="7">
         <v>11554.300000000001</v>
@@ -31666,7 +31663,7 @@
         <v>85</v>
       </c>
       <c r="E1609" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1609" s="7">
         <v>661429.36999999988</v>
@@ -31686,7 +31683,7 @@
         <v>83</v>
       </c>
       <c r="E1610" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1610" s="7">
         <v>2299269.8000000003</v>
@@ -31706,7 +31703,7 @@
         <v>87</v>
       </c>
       <c r="E1611" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1611" s="7">
         <v>25686291.770000052</v>
@@ -31726,7 +31723,7 @@
         <v>97</v>
       </c>
       <c r="E1612" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1612" s="7">
         <v>28700.580000000005</v>
@@ -31746,7 +31743,7 @@
         <v>113</v>
       </c>
       <c r="E1613" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1613" s="7">
         <v>4066416.8100000015</v>
@@ -32006,7 +32003,7 @@
         <v>105</v>
       </c>
       <c r="E1626" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1626" s="7">
         <v>634977556.71000016</v>
@@ -32066,7 +32063,7 @@
         <v>95</v>
       </c>
       <c r="E1629" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1629" s="7">
         <v>53223774.739999957</v>
@@ -32086,7 +32083,7 @@
         <v>117</v>
       </c>
       <c r="E1630" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1630" s="7">
         <v>862521.52000000025</v>
@@ -32106,7 +32103,7 @@
         <v>119</v>
       </c>
       <c r="E1631" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1631" s="7">
         <v>7867081.6499999939</v>
@@ -32126,7 +32123,7 @@
         <v>123</v>
       </c>
       <c r="E1632" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1632" s="7">
         <v>47141.71</v>
@@ -32186,7 +32183,7 @@
         <v>125</v>
       </c>
       <c r="E1635" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1635" s="7">
         <v>9880.119999999999</v>
@@ -32206,7 +32203,7 @@
         <v>135</v>
       </c>
       <c r="E1636" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1636" s="7">
         <v>518.37</v>
@@ -32226,7 +32223,7 @@
         <v>137</v>
       </c>
       <c r="E1637" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1637" s="7">
         <v>564521.81999999983</v>
@@ -32246,7 +32243,7 @@
         <v>145</v>
       </c>
       <c r="E1638" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1638" s="7">
         <v>4847388.660000002</v>
@@ -32266,7 +32263,7 @@
         <v>149</v>
       </c>
       <c r="E1639" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1639" s="7">
         <v>76015357.680000067</v>
@@ -32366,7 +32363,7 @@
         <v>151</v>
       </c>
       <c r="E1644" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1644" s="7">
         <v>39194.81</v>
@@ -32386,7 +32383,7 @@
         <v>157</v>
       </c>
       <c r="E1645" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1645" s="7">
         <v>7999.7800000000007</v>
@@ -32426,7 +32423,7 @@
         <v>161</v>
       </c>
       <c r="E1647" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1647" s="7">
         <v>470583.49000000017</v>
@@ -32446,7 +32443,7 @@
         <v>159</v>
       </c>
       <c r="E1648" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1648" s="7">
         <v>233.5</v>
@@ -32466,7 +32463,7 @@
         <v>163</v>
       </c>
       <c r="E1649" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1649" s="7">
         <v>563955987.69999945</v>
@@ -32724,7 +32721,7 @@
         <v>68</v>
       </c>
       <c r="E1662" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F1662" s="7">
         <v>781611.41</v>
@@ -32744,7 +32741,7 @@
         <v>68</v>
       </c>
       <c r="E1663" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F1663" s="7">
         <v>594151.57999999996</v>
@@ -32764,7 +32761,7 @@
         <v>68</v>
       </c>
       <c r="E1664" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F1664" s="7">
         <v>517254.38000000006</v>
@@ -32784,7 +32781,7 @@
         <v>68</v>
       </c>
       <c r="E1665" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F1665" s="7">
         <v>559530.88</v>
@@ -32804,7 +32801,7 @@
         <v>68</v>
       </c>
       <c r="E1666" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F1666" s="7">
         <v>616852.85</v>
@@ -32824,7 +32821,7 @@
         <v>68</v>
       </c>
       <c r="E1667" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F1667" s="7">
         <v>719952.25</v>
@@ -32844,7 +32841,7 @@
         <v>68</v>
       </c>
       <c r="E1668" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F1668" s="7">
         <v>912548.87</v>
@@ -33398,7 +33395,7 @@
         <v>17</v>
       </c>
       <c r="E1696" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1696" s="7">
         <v>2384757.73</v>
@@ -33418,7 +33415,7 @@
         <v>15</v>
       </c>
       <c r="E1697" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1697" s="7">
         <v>1509923.7600000002</v>
@@ -33438,7 +33435,7 @@
         <v>30</v>
       </c>
       <c r="E1698" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1698" s="7">
         <v>1363323.5800000008</v>
@@ -33458,7 +33455,7 @@
         <v>68</v>
       </c>
       <c r="E1699" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1699" s="7">
         <v>6052631.0099999998</v>
@@ -33478,7 +33475,7 @@
         <v>85</v>
       </c>
       <c r="E1700" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1700" s="7">
         <v>259421.05999999994</v>
@@ -33498,7 +33495,7 @@
         <v>145</v>
       </c>
       <c r="E1701" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1701" s="7">
         <v>4634850.8399999961</v>
@@ -33516,7 +33513,7 @@
       </c>
       <c r="D1702" s="6"/>
       <c r="E1702" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1702" s="7">
         <v>2789421770.9399981</v>
@@ -33534,7 +33531,7 @@
       </c>
       <c r="D1703" s="6"/>
       <c r="E1703" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1703" s="7">
         <v>411828484.52999961</v>
@@ -33552,7 +33549,7 @@
       </c>
       <c r="D1704" s="6"/>
       <c r="E1704" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1704" s="7">
         <v>309064093.10999995</v>
@@ -33570,13 +33567,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="14.4">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -33584,7 +33581,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30">
+    <row r="2" spans="1:2" ht="27.6">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -33592,7 +33589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="14.4">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -33600,7 +33597,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30">
+    <row r="4" spans="1:2" ht="27.6">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -33608,7 +33605,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="14.4">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -33616,7 +33613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="14.4">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -33624,7 +33621,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30">
+    <row r="7" spans="1:2" ht="27.6">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -33632,7 +33629,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="14.4">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
@@ -33640,7 +33637,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="14.4">
       <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
@@ -33648,7 +33645,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" ht="14.4">
       <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
@@ -33656,7 +33653,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="14.4">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
@@ -33664,7 +33661,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="14.4">
       <c r="A12" s="4" t="s">
         <v>29</v>
       </c>
@@ -33672,7 +33669,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="14.4">
       <c r="A13" s="4" t="s">
         <v>31</v>
       </c>
@@ -33680,7 +33677,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" ht="14.4">
       <c r="A14" s="4" t="s">
         <v>33</v>
       </c>
@@ -33688,7 +33685,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" ht="14.4">
       <c r="A15" s="4" t="s">
         <v>35</v>
       </c>
@@ -33696,7 +33693,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="14.4">
       <c r="A16" s="4" t="s">
         <v>37</v>
       </c>
@@ -33704,7 +33701,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="14.4">
       <c r="A17" s="4" t="s">
         <v>39</v>
       </c>
@@ -33712,7 +33709,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" ht="14.4">
       <c r="A18" s="4" t="s">
         <v>41</v>
       </c>
@@ -33720,7 +33717,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" ht="14.4">
       <c r="A19" s="4" t="s">
         <v>43</v>
       </c>
@@ -33728,7 +33725,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" ht="14.4">
       <c r="A20" s="4" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
fix fy disbursements download
</commit_message>
<xml_diff>
--- a/downloads/disbursements/disbursements.xlsx
+++ b/downloads/disbursements/disbursements.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malcolmj\Documents\GitHub\doi-extractives-data\gatsby-site\src\data-graphql\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goldstel\doi-extractives-data\downloads\disbursements\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$I$1704</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -908,7 +911,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -968,6 +971,9 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1251,25 +1257,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1704"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1292" workbookViewId="0">
-      <selection activeCell="H1303" sqref="H1303"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" customWidth="1"/>
-    <col min="10" max="26" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" customWidth="1"/>
+    <col min="10" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="14.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1289,7 +1295,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="14.4">
       <c r="A2" s="5">
         <v>2003</v>
       </c>
@@ -1305,7 +1311,7 @@
         <v>224798713.59999999</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="14.4">
       <c r="A3" s="5">
         <v>2003</v>
       </c>
@@ -1321,7 +1327,7 @@
         <v>150000000</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" ht="14.4">
       <c r="A4" s="5">
         <v>2003</v>
       </c>
@@ -1337,7 +1343,7 @@
         <v>898999960</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" ht="14.4">
       <c r="A5" s="5">
         <v>2003</v>
       </c>
@@ -1353,7 +1359,7 @@
         <v>753373594.29999995</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="14.4">
       <c r="A6" s="5">
         <v>2003</v>
       </c>
@@ -1371,7 +1377,7 @@
         <v>529848.84</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" ht="14.4">
       <c r="A7" s="5">
         <v>2003</v>
       </c>
@@ -1389,7 +1395,7 @@
         <v>9030501.7400000002</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" ht="14.4">
       <c r="A8" s="5">
         <v>2003</v>
       </c>
@@ -1407,7 +1413,7 @@
         <v>121898.09</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" ht="14.4">
       <c r="A9" s="5">
         <v>2003</v>
       </c>
@@ -1425,7 +1431,7 @@
         <v>4108480.76</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="14.4">
       <c r="A10" s="5">
         <v>2003</v>
       </c>
@@ -1443,7 +1449,7 @@
         <v>21837849.16</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="14.4">
       <c r="A11" s="5">
         <v>2003</v>
       </c>
@@ -1461,7 +1467,7 @@
         <v>53947136.920000002</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" ht="14.4">
       <c r="A12" s="5">
         <v>2003</v>
       </c>
@@ -1479,7 +1485,7 @@
         <v>368710.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" ht="14.4">
       <c r="A13" s="5">
         <v>2003</v>
       </c>
@@ -1497,7 +1503,7 @@
         <v>1792864.42</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="14.4">
       <c r="A14" s="5">
         <v>2003</v>
       </c>
@@ -1515,7 +1521,7 @@
         <v>109312.47</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" ht="14.4">
       <c r="A15" s="5">
         <v>2003</v>
       </c>
@@ -1533,7 +1539,7 @@
         <v>6379.25</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" ht="14.4">
       <c r="A16" s="5">
         <v>2003</v>
       </c>
@@ -1551,7 +1557,7 @@
         <v>1823378.27</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" ht="14.4">
       <c r="A17" s="5">
         <v>2003</v>
       </c>
@@ -1569,7 +1575,7 @@
         <v>50131.79</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" ht="14.4">
       <c r="A18" s="5">
         <v>2003</v>
       </c>
@@ -1587,7 +1593,7 @@
         <v>1182451.3700000001</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" ht="14.4">
       <c r="A19" s="5">
         <v>2003</v>
       </c>
@@ -1605,7 +1611,7 @@
         <v>430602.31</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" ht="14.4">
       <c r="A20" s="5">
         <v>2003</v>
       </c>
@@ -28441,8 +28447,8 @@
       <c r="B1441" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="C1441" s="19" t="s">
-        <v>255</v>
+      <c r="C1441" s="26" t="s">
+        <v>61</v>
       </c>
       <c r="D1441" s="6"/>
       <c r="E1441" s="19"/>
@@ -33559,6 +33565,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I1704"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
@@ -33570,13 +33577,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="14.4">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -33584,7 +33591,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30">
+    <row r="2" spans="1:2" ht="27.6">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -33592,7 +33599,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="14.4">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -33600,7 +33607,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30">
+    <row r="4" spans="1:2" ht="27.6">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -33608,7 +33615,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="14.4">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -33616,7 +33623,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="14.4">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -33624,7 +33631,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30">
+    <row r="7" spans="1:2" ht="27.6">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -33632,7 +33639,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="14.4">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
@@ -33640,7 +33647,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="14.4">
       <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
@@ -33648,7 +33655,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" ht="14.4">
       <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
@@ -33656,7 +33663,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="14.4">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
@@ -33664,7 +33671,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="14.4">
       <c r="A12" s="4" t="s">
         <v>29</v>
       </c>
@@ -33672,7 +33679,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="14.4">
       <c r="A13" s="4" t="s">
         <v>31</v>
       </c>
@@ -33680,7 +33687,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" ht="14.4">
       <c r="A14" s="4" t="s">
         <v>33</v>
       </c>
@@ -33688,7 +33695,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" ht="14.4">
       <c r="A15" s="4" t="s">
         <v>35</v>
       </c>
@@ -33696,7 +33703,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="14.4">
       <c r="A16" s="4" t="s">
         <v>37</v>
       </c>
@@ -33704,7 +33711,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="14.4">
       <c r="A17" s="4" t="s">
         <v>39</v>
       </c>
@@ -33712,7 +33719,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" ht="14.4">
       <c r="A18" s="4" t="s">
         <v>41</v>
       </c>
@@ -33720,7 +33727,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" ht="14.4">
       <c r="A19" s="4" t="s">
         <v>43</v>
       </c>
@@ -33728,7 +33735,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" ht="14.4">
       <c r="A20" s="4" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Attempts fix of query fails
</commit_message>
<xml_diff>
--- a/downloads/disbursements/disbursements.xlsx
+++ b/downloads/disbursements/disbursements.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goldstel\doi-extractives-data\downloads\disbursements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\doi-extractives-data\downloads\disbursements\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22992" windowHeight="9168"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$F$1833</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$F$1833</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>

</xml_diff>

<commit_message>
adds capitalization to offshore rows
</commit_message>
<xml_diff>
--- a/downloads/disbursements/disbursements.xlsx
+++ b/downloads/disbursements/disbursements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mentastc\Documents\GitHub\doi-extractives-data\downloads\disbursements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F1B6DD-B182-4842-8D75-830035F15123}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B4DA7C-392E-4497-9048-39C30C528619}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="750" windowWidth="28770" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6464" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6464" uniqueCount="256">
   <si>
     <t>Fiscal Year</t>
   </si>
@@ -438,9 +438,6 @@
   </si>
   <si>
     <t>RI</t>
-  </si>
-  <si>
-    <t>offshore</t>
   </si>
   <si>
     <t>Land &amp; Water Conservation Fund - GoMesa</t>
@@ -1667,7 +1664,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1832"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A1551" workbookViewId="0">
+      <selection activeCell="H1558" sqref="H1558"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1696,7 +1695,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -31135,7 +31134,7 @@
         <v>44</v>
       </c>
       <c r="C1561" s="4" t="s">
-        <v>138</v>
+        <v>8</v>
       </c>
       <c r="D1561" s="4" t="s">
         <v>11</v>
@@ -31153,7 +31152,7 @@
         <v>44</v>
       </c>
       <c r="C1562" s="4" t="s">
-        <v>138</v>
+        <v>8</v>
       </c>
       <c r="D1562" s="4" t="s">
         <v>12</v>
@@ -31171,7 +31170,7 @@
         <v>44</v>
       </c>
       <c r="C1563" s="4" t="s">
-        <v>138</v>
+        <v>8</v>
       </c>
       <c r="D1563" s="4" t="s">
         <v>15</v>
@@ -31189,7 +31188,7 @@
         <v>44</v>
       </c>
       <c r="C1564" s="4" t="s">
-        <v>138</v>
+        <v>8</v>
       </c>
       <c r="D1564" s="4" t="s">
         <v>23</v>
@@ -31207,7 +31206,7 @@
         <v>44</v>
       </c>
       <c r="C1565" s="4" t="s">
-        <v>138</v>
+        <v>8</v>
       </c>
       <c r="D1565" s="4" t="s">
         <v>132</v>
@@ -31225,7 +31224,7 @@
         <v>44</v>
       </c>
       <c r="C1566" s="4" t="s">
-        <v>138</v>
+        <v>8</v>
       </c>
       <c r="D1566" s="4" t="s">
         <v>26</v>
@@ -31243,7 +31242,7 @@
         <v>44</v>
       </c>
       <c r="C1567" s="4" t="s">
-        <v>138</v>
+        <v>8</v>
       </c>
       <c r="D1567" s="4" t="s">
         <v>137</v>
@@ -31261,7 +31260,7 @@
         <v>44</v>
       </c>
       <c r="C1568" s="4" t="s">
-        <v>138</v>
+        <v>8</v>
       </c>
       <c r="D1568" s="4" t="s">
         <v>39</v>
@@ -31372,7 +31371,7 @@
         <v>2018</v>
       </c>
       <c r="B1575" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C1575" s="4" t="s">
         <v>8</v>
@@ -32736,7 +32735,7 @@
         <v>6</v>
       </c>
       <c r="D1647" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E1647" s="4"/>
       <c r="F1647" s="5">
@@ -35086,7 +35085,7 @@
         <v>6</v>
       </c>
       <c r="D1770" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E1770" s="4"/>
       <c r="F1770" s="5">
@@ -36280,6 +36279,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F1832" xr:uid="{79A44272-7DF0-40AB-8085-354F7BA7DC75}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -36300,39 +36300,39 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>141</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>143</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>145</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>147</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>12</v>
@@ -36340,7 +36340,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>11</v>
@@ -36348,15 +36348,15 @@
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>151</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>14</v>
@@ -36364,15 +36364,15 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>154</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>13</v>
@@ -36380,15 +36380,15 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>157</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>15</v>
@@ -36396,15 +36396,15 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>160</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>16</v>
@@ -36412,39 +36412,39 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>163</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>165</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>167</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>169</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>17</v>
@@ -36452,39 +36452,39 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>172</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>174</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>176</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>178</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>18</v>
@@ -36492,7 +36492,7 @@
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>19</v>
@@ -36500,7 +36500,7 @@
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>20</v>
@@ -36508,7 +36508,7 @@
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>21</v>
@@ -36516,7 +36516,7 @@
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>22</v>
@@ -36524,7 +36524,7 @@
     </row>
     <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>23</v>
@@ -36532,7 +36532,7 @@
     </row>
     <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>132</v>
@@ -36540,31 +36540,31 @@
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>187</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>189</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B33" s="8" t="s">
         <v>191</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>24</v>
@@ -36572,7 +36572,7 @@
     </row>
     <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>25</v>
@@ -36580,7 +36580,7 @@
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>27</v>
@@ -36588,7 +36588,7 @@
     </row>
     <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>26</v>
@@ -36596,7 +36596,7 @@
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>28</v>
@@ -36604,23 +36604,23 @@
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="B39" s="8" t="s">
         <v>198</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="B40" s="8" t="s">
         <v>200</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>129</v>
@@ -36628,7 +36628,7 @@
     </row>
     <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>32</v>
@@ -36636,7 +36636,7 @@
     </row>
     <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>29</v>
@@ -36644,31 +36644,31 @@
     </row>
     <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B44" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="B45" s="8" t="s">
         <v>207</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="B46" s="8" t="s">
         <v>209</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>31</v>
@@ -36676,31 +36676,31 @@
     </row>
     <row r="48" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>212</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B49" s="8" t="s">
         <v>214</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B50" s="8" t="s">
         <v>216</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>30</v>
@@ -36708,15 +36708,15 @@
     </row>
     <row r="52" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B52" s="8" t="s">
         <v>219</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>33</v>
@@ -36724,7 +36724,7 @@
     </row>
     <row r="54" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>34</v>
@@ -36732,15 +36732,15 @@
     </row>
     <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B55" s="8" t="s">
         <v>223</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>35</v>
@@ -36748,7 +36748,7 @@
     </row>
     <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>36</v>
@@ -36756,31 +36756,31 @@
     </row>
     <row r="58" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B58" s="8" t="s">
         <v>227</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B59" s="8" t="s">
         <v>229</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B60" s="8" t="s">
         <v>231</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>137</v>
@@ -36788,7 +36788,7 @@
     </row>
     <row r="62" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>37</v>
@@ -36796,7 +36796,7 @@
     </row>
     <row r="63" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>38</v>
@@ -36804,15 +36804,15 @@
     </row>
     <row r="64" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="B64" s="8" t="s">
         <v>236</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>47</v>
@@ -36820,15 +36820,15 @@
     </row>
     <row r="66" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="B66" s="8" t="s">
         <v>239</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B67" s="8" t="s">
         <v>39</v>
@@ -36836,15 +36836,15 @@
     </row>
     <row r="68" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="B68" s="8" t="s">
         <v>242</v>
-      </c>
-      <c r="B68" s="8" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>40</v>
@@ -36852,7 +36852,7 @@
     </row>
     <row r="70" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>48</v>
@@ -36860,23 +36860,23 @@
     </row>
     <row r="71" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="B71" s="8" t="s">
         <v>246</v>
-      </c>
-      <c r="B71" s="8" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="B72" s="8" t="s">
         <v>248</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>41</v>
@@ -36884,15 +36884,15 @@
     </row>
     <row r="74" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B75" s="8" t="s">
         <v>42</v>
@@ -36900,7 +36900,7 @@
     </row>
     <row r="76" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B76" s="8" t="s">
         <v>43</v>
@@ -36908,10 +36908,10 @@
     </row>
     <row r="77" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B77" s="8" t="s">
         <v>254</v>
-      </c>
-      <c r="B77" s="8" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>